<commit_message>
new isha and fajr prayer times
</commit_message>
<xml_diff>
--- a/iqma-times.xlsx
+++ b/iqma-times.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaidq\Desktop\vagrant\workspace\rexdale-masjid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\rexdale-masjid\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D73868B-B6FC-45AF-9BD4-7736036EFB0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10335" xr2:uid="{23536C81-BBE2-40BC-99B3-45CC75E2F752}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28125" xr2:uid="{23536C81-BBE2-40BC-99B3-45CC75E2F752}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2607,7 +2608,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC822B9A-2A7D-44F3-B733-DDFD66B0B4CD}">
   <dimension ref="A1:L367"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A319" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M375" sqref="M375"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2689,7 +2692,7 @@
         <v>591</v>
       </c>
       <c r="L2" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2727,7 +2730,7 @@
         <v>356</v>
       </c>
       <c r="L3" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333337</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2765,7 +2768,7 @@
         <v>356</v>
       </c>
       <c r="L4" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333404</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2803,7 +2806,7 @@
         <v>355</v>
       </c>
       <c r="L5" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333404</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2841,7 +2844,7 @@
         <v>592</v>
       </c>
       <c r="L6" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333404</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2879,7 +2882,7 @@
         <v>354</v>
       </c>
       <c r="L7" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333504</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2917,7 +2920,7 @@
         <v>353</v>
       </c>
       <c r="L8" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333504</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2955,7 +2958,7 @@
         <v>593</v>
       </c>
       <c r="L9" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333504</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -2993,7 +2996,7 @@
         <v>352</v>
       </c>
       <c r="L10" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333603</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3031,7 +3034,7 @@
         <v>351</v>
       </c>
       <c r="L11" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333603</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3069,7 +3072,7 @@
         <v>594</v>
       </c>
       <c r="L12" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333603</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3107,7 +3110,7 @@
         <v>350</v>
       </c>
       <c r="L13" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333703</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3145,7 +3148,7 @@
         <v>595</v>
       </c>
       <c r="L14" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333703</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3183,7 +3186,7 @@
         <v>349</v>
       </c>
       <c r="L15" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333703</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3221,7 +3224,7 @@
         <v>348</v>
       </c>
       <c r="L16" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333803</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3259,7 +3262,7 @@
         <v>596</v>
       </c>
       <c r="L17" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333803</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3297,7 +3300,7 @@
         <v>347</v>
       </c>
       <c r="L18" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333803</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3335,7 +3338,7 @@
         <v>597</v>
       </c>
       <c r="L19" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333903</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3373,7 +3376,7 @@
         <v>346</v>
       </c>
       <c r="L20" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333903</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3411,7 +3414,7 @@
         <v>345</v>
       </c>
       <c r="L21" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333903</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3449,7 +3452,7 @@
         <v>598</v>
       </c>
       <c r="L22" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333334003</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3487,7 +3490,7 @@
         <v>599</v>
       </c>
       <c r="L23" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333334003</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3525,7 +3528,7 @@
         <v>343</v>
       </c>
       <c r="L24" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333334003</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3563,7 +3566,7 @@
         <v>342</v>
       </c>
       <c r="L25" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333334103</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3601,7 +3604,7 @@
         <v>625</v>
       </c>
       <c r="L26" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333334103</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3639,7 +3642,7 @@
         <v>341</v>
       </c>
       <c r="L27" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333334103</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3677,7 +3680,7 @@
         <v>626</v>
       </c>
       <c r="L28" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333334203</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3715,7 +3718,7 @@
         <v>627</v>
       </c>
       <c r="L29" s="1">
-        <v>0.80208333333333337</v>
+        <v>0.77083333333334203</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3753,7 +3756,7 @@
         <v>339</v>
       </c>
       <c r="L30" s="1">
-        <v>0.80208333333333337</v>
+        <v>0.77083333333334203</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3791,7 +3794,7 @@
         <v>338</v>
       </c>
       <c r="L31" s="1">
-        <v>0.80208333333333337</v>
+        <v>0.77083333333334303</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -3829,7 +3832,7 @@
         <v>628</v>
       </c>
       <c r="L32" s="1">
-        <v>0.80208333333333337</v>
+        <v>0.77083333333334303</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -14963,7 +14966,7 @@
         <v>218</v>
       </c>
       <c r="L325" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333337</v>
       </c>
     </row>
     <row r="326" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -14974,7 +14977,7 @@
         <v>28</v>
       </c>
       <c r="C326" s="1">
-        <v>0.28125</v>
+        <v>0.27083333333333298</v>
       </c>
       <c r="D326" s="4" t="s">
         <v>401</v>
@@ -15001,7 +15004,7 @@
         <v>218</v>
       </c>
       <c r="L326" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333337</v>
       </c>
     </row>
     <row r="327" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15012,7 +15015,7 @@
         <v>148</v>
       </c>
       <c r="C327" s="1">
-        <v>0.28125</v>
+        <v>0.27083333333333298</v>
       </c>
       <c r="D327" s="4" t="s">
         <v>400</v>
@@ -15039,7 +15042,7 @@
         <v>217</v>
       </c>
       <c r="L327" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="328" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15050,7 +15053,7 @@
         <v>27</v>
       </c>
       <c r="C328" s="1">
-        <v>0.28125</v>
+        <v>0.27083333333333298</v>
       </c>
       <c r="D328" s="4" t="s">
         <v>452</v>
@@ -15077,7 +15080,7 @@
         <v>217</v>
       </c>
       <c r="L328" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="329" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15088,7 +15091,7 @@
         <v>25</v>
       </c>
       <c r="C329" s="1">
-        <v>0.28125</v>
+        <v>0.27083333333333298</v>
       </c>
       <c r="D329" s="4" t="s">
         <v>398</v>
@@ -15115,7 +15118,7 @@
         <v>216</v>
       </c>
       <c r="L329" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="330" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15126,7 +15129,7 @@
         <v>24</v>
       </c>
       <c r="C330" s="1">
-        <v>0.28125</v>
+        <v>0.27083333333333298</v>
       </c>
       <c r="D330" s="4" t="s">
         <v>397</v>
@@ -15153,7 +15156,7 @@
         <v>216</v>
       </c>
       <c r="L330" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="331" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15164,7 +15167,7 @@
         <v>48</v>
       </c>
       <c r="C331" s="1">
-        <v>0.28125</v>
+        <v>0.27083333333333298</v>
       </c>
       <c r="D331" s="4" t="s">
         <v>448</v>
@@ -15191,7 +15194,7 @@
         <v>215</v>
       </c>
       <c r="L331" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="332" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15229,7 +15232,7 @@
         <v>215</v>
       </c>
       <c r="L332" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="333" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15267,7 +15270,7 @@
         <v>589</v>
       </c>
       <c r="L333" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="334" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15305,7 +15308,7 @@
         <v>589</v>
       </c>
       <c r="L334" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="335" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15343,7 +15346,7 @@
         <v>589</v>
       </c>
       <c r="L335" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="336" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15381,7 +15384,7 @@
         <v>589</v>
       </c>
       <c r="L336" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="337" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15419,7 +15422,7 @@
         <v>214</v>
       </c>
       <c r="L337" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="338" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15457,7 +15460,7 @@
         <v>214</v>
       </c>
       <c r="L338" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="339" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15495,7 +15498,7 @@
         <v>214</v>
       </c>
       <c r="L339" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="340" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15533,7 +15536,7 @@
         <v>214</v>
       </c>
       <c r="L340" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="341" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15571,7 +15574,7 @@
         <v>214</v>
       </c>
       <c r="L341" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="342" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15609,7 +15612,7 @@
         <v>214</v>
       </c>
       <c r="L342" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="343" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15647,7 +15650,7 @@
         <v>214</v>
       </c>
       <c r="L343" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="344" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15685,7 +15688,7 @@
         <v>214</v>
       </c>
       <c r="L344" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="345" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15723,7 +15726,7 @@
         <v>214</v>
       </c>
       <c r="L345" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="346" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15761,7 +15764,7 @@
         <v>214</v>
       </c>
       <c r="L346" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="347" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15799,7 +15802,7 @@
         <v>214</v>
       </c>
       <c r="L347" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="348" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15837,7 +15840,7 @@
         <v>214</v>
       </c>
       <c r="L348" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="349" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15875,7 +15878,7 @@
         <v>214</v>
       </c>
       <c r="L349" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="350" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15913,7 +15916,7 @@
         <v>589</v>
       </c>
       <c r="L350" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="351" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15951,7 +15954,7 @@
         <v>589</v>
       </c>
       <c r="L351" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="352" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -15989,7 +15992,7 @@
         <v>589</v>
       </c>
       <c r="L352" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="353" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16027,7 +16030,7 @@
         <v>215</v>
       </c>
       <c r="L353" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="354" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16065,7 +16068,7 @@
         <v>215</v>
       </c>
       <c r="L354" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="355" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16103,7 +16106,7 @@
         <v>215</v>
       </c>
       <c r="L355" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="356" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16141,7 +16144,7 @@
         <v>216</v>
       </c>
       <c r="L356" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="357" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16179,7 +16182,7 @@
         <v>216</v>
       </c>
       <c r="L357" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="358" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16217,7 +16220,7 @@
         <v>217</v>
       </c>
       <c r="L358" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="359" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16255,7 +16258,7 @@
         <v>217</v>
       </c>
       <c r="L359" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="360" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16293,7 +16296,7 @@
         <v>218</v>
       </c>
       <c r="L360" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="361" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16331,7 +16334,7 @@
         <v>360</v>
       </c>
       <c r="L361" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="362" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16369,7 +16372,7 @@
         <v>360</v>
       </c>
       <c r="L362" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="363" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16407,7 +16410,7 @@
         <v>359</v>
       </c>
       <c r="L363" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="364" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16445,7 +16448,7 @@
         <v>590</v>
       </c>
       <c r="L364" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="365" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16483,7 +16486,7 @@
         <v>590</v>
       </c>
       <c r="L365" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="366" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16521,7 +16524,7 @@
         <v>358</v>
       </c>
       <c r="L366" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333304</v>
       </c>
     </row>
     <row r="367" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -16559,7 +16562,7 @@
         <v>357</v>
       </c>
       <c r="L367" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.77083333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>